<commit_message>
added updated excelfile to have different area post codes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/postalCode.xlsx
+++ b/src/test/resources/TestData/postalCode.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\TestNG\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonam\Desktop\Workspace\SeleniumTestng\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B410D8CC-0D65-43A6-BDE1-39C18F8742F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C009A6B5-EE34-4BB9-99C0-C76E2F971476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C3D9DF37-C3CB-459E-A867-D02BA7CF1E16}"/>
   </bookViews>
@@ -42,34 +42,34 @@
     <t>M1 1PW</t>
   </si>
   <si>
-    <t>M1 1PL</t>
-  </si>
-  <si>
-    <t>M1 1PX</t>
-  </si>
-  <si>
     <t>M1 1JQ</t>
   </si>
   <si>
-    <t>M1 1BY</t>
-  </si>
-  <si>
     <t>M1 1AD</t>
   </si>
   <si>
-    <t>M1 1FN</t>
-  </si>
-  <si>
-    <t>M1 1LU</t>
-  </si>
-  <si>
     <t>M1 4DZ</t>
   </si>
   <si>
-    <t>M1 3BE</t>
-  </si>
-  <si>
-    <t>M1 2PY</t>
+    <t>L1 3HD</t>
+  </si>
+  <si>
+    <t>L1 5AS</t>
+  </si>
+  <si>
+    <t>EX17 3AH</t>
+  </si>
+  <si>
+    <t>HA8 7JL</t>
+  </si>
+  <si>
+    <t>S70 1RU</t>
+  </si>
+  <si>
+    <t>B17 9NP</t>
+  </si>
+  <si>
+    <t>TR18 2TN</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,52 +441,52 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>